<commit_message>
Multiple figures added, all figures were polished or updated in some way. Streamlined some of the code that didn't make sense. Added dplyr:: calls to mutate and summarise to prevent errors.
</commit_message>
<xml_diff>
--- a/data/Microcystis Quota Estimates.xlsx
+++ b/data/Microcystis Quota Estimates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanbaker/Desktop/NOAA_Omics_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylanbaker/Desktop/mLife2023Baker/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA9C118E-A246-6B44-B157-992C4CB49A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E794D4-F412-9F4E-8929-0842B682A84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="4400" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="9440" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -324,7 +324,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="149">
   <si>
     <t>Date</t>
   </si>
@@ -698,16 +698,10 @@
     <t>ks_P</t>
   </si>
   <si>
-    <t>Qp</t>
-  </si>
-  <si>
     <t>mumax_N</t>
   </si>
   <si>
     <t>ks_N</t>
-  </si>
-  <si>
-    <t>Qn</t>
   </si>
   <si>
     <t>P&lt;sup&gt;*&lt;sup&gt;, d = 0.2 day&lt;sup&gt;-1&lt;/sup&gt;</t>
@@ -717,6 +711,66 @@
   </si>
   <si>
     <t>Do between strain</t>
+  </si>
+  <si>
+    <t>sig_ksP</t>
+  </si>
+  <si>
+    <t>sig_mumaxP</t>
+  </si>
+  <si>
+    <t>sig_ksN</t>
+  </si>
+  <si>
+    <t>sig_mumaxN</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>ns</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Axenic</t>
+  </si>
+  <si>
+    <t>Xenic</t>
+  </si>
+  <si>
+    <t>NIES-843</t>
+  </si>
+  <si>
+    <t>PCC 7806 ΔmcyB</t>
+  </si>
+  <si>
+    <t>PCC 7806</t>
+  </si>
+  <si>
+    <t>PCC 9701</t>
+  </si>
+  <si>
+    <t>Q_P</t>
+  </si>
+  <si>
+    <t>Q_N</t>
+  </si>
+  <si>
+    <t>mumax_P_SE</t>
+  </si>
+  <si>
+    <t>ks_P_SE</t>
+  </si>
+  <si>
+    <t>mumax_N_SE</t>
+  </si>
+  <si>
+    <t>ks_N_SE</t>
   </si>
 </sst>
 </file>
@@ -731,7 +785,7 @@
     <numFmt numFmtId="168" formatCode="0.000000"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,6 +835,13 @@
       <color theme="1"/>
       <name val="Helvetica"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -846,7 +907,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -907,6 +968,7 @@
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1125,7 +1187,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BQ1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="AP1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="A12" sqref="A12:XFD16"/>
     </sheetView>
@@ -3436,7 +3498,7 @@
       <c r="I20" s="22"/>
       <c r="J20" s="22"/>
       <c r="K20" s="42" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L20" s="23"/>
       <c r="BB20" s="23"/>
@@ -15237,8 +15299,8 @@
   </sheetPr>
   <dimension ref="A1:AI81"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15276,7 +15338,7 @@
         <v>84</v>
       </c>
       <c r="F1" s="45" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>91</v>
@@ -15291,7 +15353,7 @@
         <v>85</v>
       </c>
       <c r="K1" s="46" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L1" s="32" t="s">
         <v>86</v>
@@ -15936,225 +15998,423 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88A4B1D5-101C-4A4D-AE53-A7B30166C909}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="F1" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="G1" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="K1" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="L1" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="M1" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="F1" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="25" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="N1" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="O1" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2">
+        <v>140</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2">
         <v>0.55261318999999998</v>
       </c>
-      <c r="C2">
+      <c r="D2">
+        <v>0.01</v>
+      </c>
+      <c r="F2">
         <v>3.58498312</v>
       </c>
-      <c r="D2">
+      <c r="G2" s="50">
+        <v>0.75</v>
+      </c>
+      <c r="I2">
         <v>1.269892</v>
       </c>
-      <c r="E2">
+      <c r="J2">
         <v>0.59851365999999995</v>
       </c>
-      <c r="F2">
+      <c r="K2" s="25">
+        <v>0.04</v>
+      </c>
+      <c r="M2">
         <v>290.57953258999999</v>
       </c>
-      <c r="G2">
+      <c r="N2" s="25">
+        <v>100.11</v>
+      </c>
+      <c r="P2">
         <v>28.857124373192608</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3">
         <v>0.49354604000000002</v>
       </c>
-      <c r="C3">
+      <c r="D3">
+        <v>0.01</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F3">
         <v>1.71552134</v>
       </c>
-      <c r="D3">
+      <c r="G3" s="50">
+        <v>0.42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3">
         <v>0.85024500000000003</v>
       </c>
-      <c r="E3">
+      <c r="J3">
         <v>0.47352663</v>
       </c>
-      <c r="F3">
+      <c r="K3" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="L3" t="s">
+        <v>134</v>
+      </c>
+      <c r="M3">
         <v>66.757095399999997</v>
       </c>
-      <c r="G3">
+      <c r="N3" s="25">
+        <v>25.29</v>
+      </c>
+      <c r="O3" t="s">
+        <v>134</v>
+      </c>
+      <c r="P3">
         <v>48.220093955177489</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4">
+        <v>141</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C4">
         <v>0.47940885999999999</v>
       </c>
-      <c r="C4">
+      <c r="D4">
+        <v>0.01</v>
+      </c>
+      <c r="F4">
         <v>0.91863576999999996</v>
       </c>
-      <c r="D4">
+      <c r="G4" s="50">
+        <v>0.16</v>
+      </c>
+      <c r="I4">
         <v>0.87520600000000004</v>
       </c>
-      <c r="E4">
+      <c r="J4">
         <v>0.58334615999999995</v>
       </c>
-      <c r="F4">
+      <c r="K4" s="25">
+        <v>0.04</v>
+      </c>
+      <c r="M4">
         <v>233.13164273000001</v>
       </c>
-      <c r="G4">
+      <c r="N4" s="25">
+        <v>83.95</v>
+      </c>
+      <c r="P4">
         <v>48.098719100125038</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C5">
         <v>0.46743717000000001</v>
       </c>
-      <c r="C5">
+      <c r="D5">
+        <v>0.01</v>
+      </c>
+      <c r="E5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F5">
         <v>0.62740702999999998</v>
       </c>
-      <c r="D5">
+      <c r="G5" s="50">
+        <v>0.12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I5">
         <v>0.71563100000000002</v>
       </c>
-      <c r="E5">
+      <c r="J5">
         <v>0.42607685000000001</v>
       </c>
-      <c r="F5">
+      <c r="K5" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="L5" t="s">
+        <v>133</v>
+      </c>
+      <c r="M5">
         <v>63.280025010000003</v>
       </c>
-      <c r="G5">
+      <c r="N5" s="25">
+        <v>27.84</v>
+      </c>
+      <c r="O5" t="s">
+        <v>135</v>
+      </c>
+      <c r="P5">
         <v>44.888032763902238</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6">
+        <v>142</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6">
         <v>0.53665288</v>
       </c>
-      <c r="C6">
+      <c r="D6">
+        <v>0.02</v>
+      </c>
+      <c r="F6">
         <v>5.3513131999999999</v>
       </c>
-      <c r="D6">
+      <c r="G6" s="50">
+        <v>1.34</v>
+      </c>
+      <c r="I6">
         <v>1.890333</v>
       </c>
-      <c r="E6">
+      <c r="J6">
         <v>0.57745837</v>
       </c>
-      <c r="F6">
+      <c r="K6" s="34">
+        <v>0.03</v>
+      </c>
+      <c r="M6">
         <v>342.09716493000002</v>
       </c>
-      <c r="G6">
+      <c r="N6" s="25">
+        <v>112.68</v>
+      </c>
+      <c r="P6">
         <v>94.157133928072739</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7">
+        <v>142</v>
+      </c>
+      <c r="B7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7">
         <v>0.58480328999999998</v>
       </c>
-      <c r="C7">
+      <c r="D7">
+        <v>0.02</v>
+      </c>
+      <c r="E7" t="s">
+        <v>135</v>
+      </c>
+      <c r="F7">
         <v>7.1075060499999996</v>
       </c>
-      <c r="D7">
+      <c r="G7" s="50">
+        <v>1.5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>135</v>
+      </c>
+      <c r="I7">
         <v>3.4139400000000002</v>
       </c>
-      <c r="E7">
+      <c r="J7">
         <v>0.57953213999999997</v>
       </c>
-      <c r="F7">
+      <c r="K7" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="L7" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7">
         <v>133.63828927</v>
       </c>
-      <c r="G7">
+      <c r="N7" s="25">
+        <v>39.25</v>
+      </c>
+      <c r="O7" t="s">
+        <v>135</v>
+      </c>
+      <c r="P7">
         <v>157.43766245406945</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8">
+        <v>139</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8">
         <v>0.53964193999999999</v>
       </c>
-      <c r="C8">
+      <c r="D8">
+        <v>0.01</v>
+      </c>
+      <c r="F8">
         <v>4.0096336299999997</v>
       </c>
-      <c r="D8">
+      <c r="G8" s="50">
+        <v>0.9</v>
+      </c>
+      <c r="I8">
         <v>3.2375069999999999</v>
       </c>
-      <c r="E8">
+      <c r="J8">
         <v>0.53681166999999996</v>
       </c>
-      <c r="F8">
+      <c r="K8" s="25">
+        <v>0.03</v>
+      </c>
+      <c r="M8">
         <v>371.77858719</v>
       </c>
-      <c r="G8">
+      <c r="N8" s="25">
+        <v>92.89</v>
+      </c>
+      <c r="P8">
         <v>53.330997650974808</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9">
+        <v>139</v>
+      </c>
+      <c r="B9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9">
         <v>0.54778402999999998</v>
       </c>
-      <c r="C9">
+      <c r="D9">
+        <v>0.01</v>
+      </c>
+      <c r="E9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F9">
         <v>3.9378301699999998</v>
       </c>
-      <c r="D9">
+      <c r="G9" s="50">
+        <v>0.87</v>
+      </c>
+      <c r="H9" t="s">
+        <v>135</v>
+      </c>
+      <c r="I9">
         <v>2.611081</v>
       </c>
-      <c r="E9">
+      <c r="J9">
         <v>0.47965622000000002</v>
       </c>
-      <c r="F9">
+      <c r="K9" s="25">
+        <v>0.02</v>
+      </c>
+      <c r="L9" t="s">
+        <v>135</v>
+      </c>
+      <c r="M9">
         <v>121.4402652</v>
       </c>
-      <c r="G9">
+      <c r="N9" s="25">
+        <v>29.81</v>
+      </c>
+      <c r="O9" t="s">
+        <v>134</v>
+      </c>
+      <c r="P9">
         <v>55.122246771368097</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>